<commit_message>
DataProcess: Fixed Issue where the lo and hi bytes for conversion were being used incorrectly
Packet Calcs.xlsx:
Added cost calculation for fligth duration and resending
</commit_message>
<xml_diff>
--- a/PacketCalcs.xlsx
+++ b/PacketCalcs.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Collin\Desktop\Research\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Collin\Desktop\Research\Repo\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>Packet size MAX</t>
   </si>
@@ -112,6 +112,24 @@
   </si>
   <si>
     <t>Number of Reading cycle that fit</t>
+  </si>
+  <si>
+    <t>Temp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Time </t>
+  </si>
+  <si>
+    <t>Size</t>
+  </si>
+  <si>
+    <t>Cost per packet</t>
+  </si>
+  <si>
+    <t>Cost for all data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cost with resending </t>
   </si>
 </sst>
 </file>
@@ -429,10 +447,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J18"/>
+  <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -457,7 +475,7 @@
       </c>
       <c r="B2">
         <f>J6</f>
-        <v>1934</v>
+        <v>1936</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -465,8 +483,8 @@
         <v>16</v>
       </c>
       <c r="J4">
-        <f>B1-C18</f>
-        <v>1958</v>
+        <f>B1-C21</f>
+        <v>1956</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -474,8 +492,8 @@
         <v>28</v>
       </c>
       <c r="J5">
-        <f>_xlfn.FLOOR.MATH(J4/E12)</f>
-        <v>46</v>
+        <f>_xlfn.FLOOR.MATH(J4/E14)</f>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -483,8 +501,8 @@
         <v>27</v>
       </c>
       <c r="J6">
-        <f>C18+J5*E12</f>
-        <v>1934</v>
+        <f>C21+J5*E14</f>
+        <v>1936</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -563,67 +581,115 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="B11">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C11">
         <v>16</v>
       </c>
       <c r="D11">
-        <f>C11/8</f>
         <v>2</v>
       </c>
       <c r="E11">
         <f>B11*D11</f>
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <v>3</v>
+      </c>
+      <c r="C12">
+        <v>16</v>
+      </c>
+      <c r="D12">
+        <f>C12/8</f>
+        <v>2</v>
+      </c>
+      <c r="E12">
+        <f>B12*D12</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>16</v>
+      </c>
+      <c r="D13">
+        <f>C13/8</f>
+        <v>2</v>
+      </c>
+      <c r="E13">
+        <f>B13*D13</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>17</v>
       </c>
-      <c r="E12">
-        <f>SUM(E8:E11)</f>
-        <v>42</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>12</v>
-      </c>
-      <c r="B16" t="s">
-        <v>13</v>
-      </c>
-      <c r="C16" t="s">
-        <v>14</v>
+      <c r="E14">
+        <f>SUM(E8:E13)</f>
+        <v>46</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>15</v>
-      </c>
-      <c r="B17">
-        <v>16</v>
-      </c>
-      <c r="C17">
-        <f>B17/8</f>
-        <v>2</v>
+        <v>11</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>12</v>
+      </c>
+      <c r="B18" t="s">
+        <v>13</v>
+      </c>
+      <c r="C18" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>31</v>
+      </c>
+      <c r="B19">
+        <v>16</v>
+      </c>
+      <c r="C19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>15</v>
+      </c>
+      <c r="B20">
+        <v>16</v>
+      </c>
+      <c r="C20">
+        <f>B20/8</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>18</v>
       </c>
-      <c r="C18">
-        <f>SUM(C17)</f>
-        <v>2</v>
+      <c r="C21">
+        <f>SUM(C19:C20)</f>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -633,15 +699,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="9" max="9" width="13.140625" customWidth="1"/>
+    <col min="10" max="10" width="17.42578125" customWidth="1"/>
+    <col min="11" max="11" width="12.85546875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>19</v>
       </c>
@@ -649,39 +720,60 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2">
         <f>'Packet Calculations'!J5</f>
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="F2">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>20</v>
       </c>
       <c r="F4" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I4" t="s">
+        <v>32</v>
+      </c>
+      <c r="J4" t="s">
+        <v>33</v>
+      </c>
+      <c r="K4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5">
         <f>'Packet Calculations'!B8/3 * 100</f>
         <v>400</v>
       </c>
       <c r="F5">
         <f>_xlfn.CEILING.MATH(F2/A11)</f>
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+      <c r="I5">
+        <f>0.04 + 0.0015 * ('Packet Calculations'!J6-'Packet Calculations'!D23-30)</f>
+        <v>2.899</v>
+      </c>
+      <c r="J5">
+        <f>I5*F5</f>
+        <v>60.878999999999998</v>
+      </c>
+      <c r="K5">
+        <f>J5*3</f>
+        <v>182.637</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="F7" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -689,13 +781,13 @@
         <v>64000</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9">
         <f>A5*A2</f>
-        <v>18400</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+        <v>16800</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -703,10 +795,10 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11">
         <f>A9/1000</f>
-        <v>18.399999999999999</v>
+        <v>16.8</v>
       </c>
       <c r="F11">
         <f>IF(F8-(F5*'Packet Calculations'!B2) &gt; 0, 1, 0)</f>

</xml_diff>